<commit_message>
updates data.json and report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#200000SWHCGMXX/COMPUGROUP_MEDICAL_ITALIA_S.p.a/CCBASIC/3.36/report-checklist.xlsx
+++ b/GATEWAY/A1#200000SWHCGMXX/COMPUGROUP_MEDICAL_ITALIA_S.p.a/CCBASIC/3.36/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/domenico_depinto_cgm_com/Documents/validazione_sogei/A1#200000SWHCGMXX/COMPUGROUP_MEDICAL_ITALIA_S.p.a/CCBASIC/3.36/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_D02697B058064E8558B1D8CE05CFACF2181887E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{813E6C69-F328-4AFA-9AC0-80AC657A3673}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="11_D02697B058064E8558B1D8CE05CFACF2181887E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00F499F0-446D-44C9-B2C9-E778CEF14C46}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="192">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -821,12 +821,6 @@
     <t>subject_application_version: 3.36</t>
   </si>
   <si>
-    <t>il nostro gestionale non gestisce la sezione Piani di Cura</t>
-  </si>
-  <si>
-    <t>il nostro gestionale non gestisce le sezioni Piani di Cura e Reti di patologia</t>
-  </si>
-  <si>
     <t>JWT payload: non è stato possibile verificare il codice fiscale del paziente presente nel CDA</t>
   </si>
   <si>
@@ -851,24 +845,6 @@
     <t>2.16.840.1.113883.2.9.2.190201.4.4.f3fb1c67aa04f48efdaa83e06f44e75bab4dc02713d769239b0742fe6f3deea7.d711beac04^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-10-24T12:10:44Z</t>
-  </si>
-  <si>
-    <t>a221cd7a22cc0dbe</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190201.4.4.9a3f0693f652f3b295bfd1ab27c2ce672bc725f7202b0784825912ccc6ebcb82.73f997e09e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-24T12:13:27Z</t>
-  </si>
-  <si>
-    <t>0d6582c60acadadf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190201.4.4.b9c8afb97cf681c3e18f85404126c2ff9eb61bc781e2f4ed6a0fb85c3884b08f.a8ab0abcd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-10-24T12:14:52Z</t>
   </si>
   <si>
@@ -878,22 +854,7 @@
     <t>2.16.840.1.113883.2.9.2.190201.4.4.d56f5abcc766e5436de70e80b05f889569b9f4f25ad3de25e08b812c4e54b53b.a0e4ce9298^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-10-24T05:15:05Z</t>
-  </si>
-  <si>
-    <t>5c8a64ef7ae80cf1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190201.4.4.d56f5abcc766e5436de70e80b05f889569b9f4f25ad3de25e08b812c4e54b53b.c2d0fe3c14^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-24T05:15:59Z</t>
-  </si>
-  <si>
-    <t>627c1eca4b08e705</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190201.4.4.9677814f1b2c6ca66759b04545078dc599eb0bc1e3cded300bfa9d4abb110784.656a8b5f16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>il nostro gestionale non gestisce le sezioni Piani di Cura, Reti di patologia e annotazioni</t>
   </si>
 </sst>
 </file>
@@ -3841,10 +3802,10 @@
   <dimension ref="A1:T651"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P18" sqref="P18"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4202,11 +4163,11 @@
         <v>60</v>
       </c>
       <c r="N12" s="39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O12" s="38"/>
       <c r="P12" s="38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q12" s="38"/>
       <c r="R12" s="40" t="s">
@@ -4233,22 +4194,16 @@
       <c r="E13" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="27">
-        <v>45223</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="H13" s="28" t="s">
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K13" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="I13" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="J13" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="29"/>
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
@@ -4277,22 +4232,16 @@
       <c r="E14" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="27">
-        <v>45223</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>195</v>
-      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" s="29"/>
+        <v>159</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>191</v>
+      </c>
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
       <c r="N14" s="29"/>
@@ -4300,9 +4249,7 @@
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
       <c r="R14" s="30"/>
-      <c r="S14" s="29" t="s">
-        <v>180</v>
-      </c>
+      <c r="S14" s="29"/>
       <c r="T14" s="32" t="s">
         <v>46</v>
       </c>
@@ -4323,22 +4270,16 @@
       <c r="E15" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="27">
-        <v>45223</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="H15" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>201</v>
-      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="K15" s="29"/>
+        <v>159</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>191</v>
+      </c>
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
       <c r="N15" s="29"/>
@@ -4346,9 +4287,7 @@
       <c r="P15" s="29"/>
       <c r="Q15" s="29"/>
       <c r="R15" s="30"/>
-      <c r="S15" s="29" t="s">
-        <v>180</v>
-      </c>
+      <c r="S15" s="29"/>
       <c r="T15" s="32" t="s">
         <v>46</v>
       </c>
@@ -4369,22 +4308,16 @@
       <c r="E16" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="27">
-        <v>45223</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H16" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>204</v>
-      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
       <c r="J16" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="29"/>
+        <v>159</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>191</v>
+      </c>
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
       <c r="N16" s="29"/>
@@ -4392,9 +4325,7 @@
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
       <c r="R16" s="30"/>
-      <c r="S16" s="29" t="s">
-        <v>181</v>
-      </c>
+      <c r="S16" s="29"/>
       <c r="T16" s="32" t="s">
         <v>46</v>
       </c>
@@ -4457,13 +4388,13 @@
         <v>45223</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="J18" s="29" t="s">
         <v>60</v>
@@ -4476,13 +4407,13 @@
         <v>60</v>
       </c>
       <c r="N18" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O18" s="29" t="s">
         <v>159</v>
       </c>
       <c r="P18" s="29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
@@ -4857,7 +4788,7 @@
         <v>159</v>
       </c>
       <c r="K28" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L28" s="29"/>
       <c r="M28" s="29"/>
@@ -5081,13 +5012,13 @@
         <v>45223</v>
       </c>
       <c r="G34" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="I34" s="28" t="s">
         <v>187</v>
-      </c>
-      <c r="H34" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="I34" s="28" t="s">
-        <v>189</v>
       </c>
       <c r="J34" s="29" t="s">
         <v>60</v>

</xml_diff>